<commit_message>
backup de todos os fontes
</commit_message>
<xml_diff>
--- a/Acompanhamento de tarefas.xlsx
+++ b/Acompanhamento de tarefas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="165">
   <si>
     <t>Tarefas CCBA</t>
   </si>
@@ -502,6 +502,18 @@
   </si>
   <si>
     <t>PRECISA QUE SEJA CRIADO UMA ROTINA, PARA DEIXAR ADICIONAR/ALTERAR O HISTÓRICO DO PEDIDO DE VENDA, MESMO QUANDO JÁ TENHA FATURADO. PERMISSÃO DEVE SER COLOCADA APENAS PARA MARISA.</t>
+  </si>
+  <si>
+    <t>AJUSTAR RELATÓRIO ADICIONANDO MAIS 4 CAMPOS, PARA QUE SEJA EXPORTADO PARA EXCEL. DEVERÁ SER FEITO TANTO PARA RELEASE 3 E 4;</t>
+  </si>
+  <si>
+    <t>RMATR680B</t>
+  </si>
+  <si>
+    <t>AJUSTAR  PONTO DE ENTRADA SF1100I ENCONTRO DE CONTAS QUE NÃO ESTÁ COM A NOVA REGRA DETERMINADA PELO ANTONIO. DEVERÁ RESPEITAR A OPÇÃO SELECIONADA NO PEDIDO DE COMPRAS;</t>
+  </si>
+  <si>
+    <t>SF1100I</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1175,133 @@
     <cellStyle name="Título" xfId="1" builtinId="15"/>
     <cellStyle name="Total" xfId="5" builtinId="25"/>
   </cellStyles>
-  <dxfs count="162">
+  <dxfs count="180">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2604,11 +2742,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan1"/>
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51:E52"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2653,7 +2791,7 @@
       </c>
       <c r="J2" s="78">
         <f>COUNTIF(G6:G112,2)</f>
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3751,7 +3889,7 @@
     </row>
     <row r="41" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A41" s="65">
-        <f t="shared" ref="A41:A48" si="4">A40+1</f>
+        <f t="shared" ref="A41:A50" si="4">A40+1</f>
         <v>34</v>
       </c>
       <c r="B41" s="73" t="s">
@@ -3986,6 +4124,66 @@
         <v>41411</v>
       </c>
       <c r="I48" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A49" s="65">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="B49" s="73" t="s">
+        <v>161</v>
+      </c>
+      <c r="C49" s="67">
+        <v>41421</v>
+      </c>
+      <c r="D49" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="E49" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="F49" s="72" t="s">
+        <v>162</v>
+      </c>
+      <c r="G49" s="69">
+        <v>2</v>
+      </c>
+      <c r="H49" s="70">
+        <v>41421</v>
+      </c>
+      <c r="I49" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="65">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="B50" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="C50" s="67">
+        <v>41423</v>
+      </c>
+      <c r="D50" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="E50" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="F50" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="G50" s="69">
+        <v>2</v>
+      </c>
+      <c r="H50" s="70">
+        <v>41423</v>
+      </c>
+      <c r="I50" s="71">
         <v>0</v>
       </c>
     </row>
@@ -3995,7 +4193,7 @@
     <mergeCell ref="B2:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="H2">
-    <cfRule type="iconSet" priority="225">
+    <cfRule type="iconSet" priority="239">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4004,7 +4202,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="iconSet" priority="224">
+    <cfRule type="iconSet" priority="238">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4013,7 +4211,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="iconSet" priority="223">
+    <cfRule type="iconSet" priority="237">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4022,7 +4220,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="iconSet" priority="221">
+    <cfRule type="iconSet" priority="235">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4031,15 +4229,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:I6 B7:I7 A25:I26 A39:A41 A37:I37">
-    <cfRule type="expression" dxfId="161" priority="219">
+    <cfRule type="expression" dxfId="179" priority="233">
       <formula>$G6=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="220">
+    <cfRule type="expression" dxfId="178" priority="234">
       <formula>$G6=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="iconSet" priority="218">
+    <cfRule type="iconSet" priority="232">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4048,15 +4246,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:I12">
-    <cfRule type="expression" dxfId="159" priority="216">
+    <cfRule type="expression" dxfId="177" priority="230">
       <formula>$G12=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="217">
+    <cfRule type="expression" dxfId="176" priority="231">
       <formula>$G12=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13">
-    <cfRule type="iconSet" priority="215">
+    <cfRule type="iconSet" priority="229">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4065,15 +4263,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:I13">
-    <cfRule type="expression" dxfId="157" priority="213">
+    <cfRule type="expression" dxfId="175" priority="227">
       <formula>$G13=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="214">
+    <cfRule type="expression" dxfId="174" priority="228">
       <formula>$G13=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="iconSet" priority="212">
+    <cfRule type="iconSet" priority="226">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4082,15 +4280,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:I14">
-    <cfRule type="expression" dxfId="155" priority="210">
+    <cfRule type="expression" dxfId="173" priority="224">
       <formula>$G14=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="211">
+    <cfRule type="expression" dxfId="172" priority="225">
       <formula>$G14=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15">
-    <cfRule type="iconSet" priority="206">
+    <cfRule type="iconSet" priority="220">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4099,15 +4297,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:I15">
-    <cfRule type="expression" dxfId="153" priority="204">
+    <cfRule type="expression" dxfId="171" priority="218">
       <formula>$G15=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="205">
+    <cfRule type="expression" dxfId="170" priority="219">
       <formula>$G15=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="iconSet" priority="203">
+    <cfRule type="iconSet" priority="217">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4116,15 +4314,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:I17">
-    <cfRule type="expression" dxfId="151" priority="201">
+    <cfRule type="expression" dxfId="169" priority="215">
       <formula>$G17=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="202">
+    <cfRule type="expression" dxfId="168" priority="216">
       <formula>$G17=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G22">
-    <cfRule type="iconSet" priority="197">
+    <cfRule type="iconSet" priority="211">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4133,15 +4331,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:I22">
-    <cfRule type="expression" dxfId="149" priority="195">
+    <cfRule type="expression" dxfId="167" priority="209">
       <formula>$G19=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="196">
+    <cfRule type="expression" dxfId="166" priority="210">
       <formula>$G19=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="iconSet" priority="194">
+    <cfRule type="iconSet" priority="208">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4150,15 +4348,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:I18">
-    <cfRule type="expression" dxfId="147" priority="192">
+    <cfRule type="expression" dxfId="165" priority="206">
       <formula>$G18=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="193">
+    <cfRule type="expression" dxfId="164" priority="207">
       <formula>$G18=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28 G23:G26">
-    <cfRule type="iconSet" priority="191">
+    <cfRule type="iconSet" priority="205">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4167,15 +4365,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:I24 B28:I28">
-    <cfRule type="expression" dxfId="145" priority="189">
+    <cfRule type="expression" dxfId="163" priority="203">
       <formula>$G23=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="190">
+    <cfRule type="expression" dxfId="162" priority="204">
       <formula>$G23=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29:G30">
-    <cfRule type="iconSet" priority="188">
+    <cfRule type="iconSet" priority="202">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4184,15 +4382,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:I30">
-    <cfRule type="expression" dxfId="143" priority="186">
+    <cfRule type="expression" dxfId="161" priority="200">
       <formula>$G29=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="187">
+    <cfRule type="expression" dxfId="160" priority="201">
       <formula>$G29=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31">
-    <cfRule type="iconSet" priority="185">
+    <cfRule type="iconSet" priority="199">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4201,14 +4399,72 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:I31">
-    <cfRule type="expression" dxfId="141" priority="183">
+    <cfRule type="expression" dxfId="159" priority="197">
       <formula>$G31=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="184">
+    <cfRule type="expression" dxfId="158" priority="198">
       <formula>$G31=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
+    <cfRule type="iconSet" priority="196">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="1" gte="0"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:I32">
+    <cfRule type="expression" dxfId="157" priority="194">
+      <formula>$G32=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="156" priority="195">
+      <formula>$G32=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="expression" dxfId="155" priority="192">
+      <formula>$G32=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="154" priority="193">
+      <formula>$G32=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35 C35:F35 H35:I35">
+    <cfRule type="expression" dxfId="153" priority="189">
+      <formula>$G35=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="152" priority="190">
+      <formula>$G35=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="expression" dxfId="151" priority="187">
+      <formula>$G35=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="150" priority="188">
+      <formula>$G35=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="iconSet" priority="186">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="1" gte="0"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="expression" dxfId="149" priority="184">
+      <formula>$G35=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="148" priority="185">
+      <formula>$G35=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G39">
     <cfRule type="iconSet" priority="182">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -4217,39 +4473,23 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32:I32">
-    <cfRule type="expression" dxfId="139" priority="180">
-      <formula>$G32=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="138" priority="181">
-      <formula>$G32=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="137" priority="178">
-      <formula>$G32=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="136" priority="179">
-      <formula>$G32=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35 C35:F35 H35:I35">
-    <cfRule type="expression" dxfId="135" priority="175">
-      <formula>$G35=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="134" priority="176">
-      <formula>$G35=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B35">
-    <cfRule type="expression" dxfId="133" priority="173">
-      <formula>$G35=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="132" priority="174">
-      <formula>$G35=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
+  <conditionalFormatting sqref="C39:I39">
+    <cfRule type="expression" dxfId="147" priority="180">
+      <formula>$G39=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="146" priority="181">
+      <formula>$G39=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39">
+    <cfRule type="expression" dxfId="145" priority="178">
+      <formula>$G39=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="179">
+      <formula>$G39=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G37">
     <cfRule type="iconSet" priority="172">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -4258,16 +4498,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="expression" dxfId="131" priority="170">
-      <formula>$G35=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="130" priority="171">
-      <formula>$G35=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G39">
-    <cfRule type="iconSet" priority="168">
+  <conditionalFormatting sqref="G40">
+    <cfRule type="iconSet" priority="167">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4275,24 +4507,24 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39:I39">
-    <cfRule type="expression" dxfId="129" priority="166">
-      <formula>$G39=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="128" priority="167">
-      <formula>$G39=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
-    <cfRule type="expression" dxfId="127" priority="164">
-      <formula>$G39=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="126" priority="165">
-      <formula>$G39=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G37">
-    <cfRule type="iconSet" priority="158">
+  <conditionalFormatting sqref="C40:I40">
+    <cfRule type="expression" dxfId="143" priority="165">
+      <formula>$G40=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="142" priority="166">
+      <formula>$G40=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="expression" dxfId="141" priority="163">
+      <formula>$G40=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="164">
+      <formula>$G40=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="iconSet" priority="162">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4300,8 +4532,24 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
-    <cfRule type="iconSet" priority="153">
+  <conditionalFormatting sqref="C41:I41">
+    <cfRule type="expression" dxfId="139" priority="160">
+      <formula>$G41=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="138" priority="161">
+      <formula>$G41=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="expression" dxfId="137" priority="158">
+      <formula>$G41=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="136" priority="159">
+      <formula>$G41=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="iconSet" priority="157">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4309,24 +4557,40 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40:I40">
-    <cfRule type="expression" dxfId="125" priority="151">
-      <formula>$G40=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="124" priority="152">
-      <formula>$G40=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="123" priority="149">
-      <formula>$G40=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="122" priority="150">
-      <formula>$G40=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G41">
-    <cfRule type="iconSet" priority="148">
+  <conditionalFormatting sqref="A13">
+    <cfRule type="expression" dxfId="135" priority="153">
+      <formula>$G13=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="134" priority="154">
+      <formula>$G13=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15 A17:A24 A28">
+    <cfRule type="expression" dxfId="133" priority="151">
+      <formula>$G15=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="132" priority="152">
+      <formula>$G15=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="expression" dxfId="131" priority="149">
+      <formula>$G32=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="130" priority="150">
+      <formula>$G32=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="expression" dxfId="129" priority="140">
+      <formula>$G9=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="128" priority="141">
+      <formula>$G9=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="iconSet" priority="139">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4334,24 +4598,48 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41:I41">
-    <cfRule type="expression" dxfId="121" priority="146">
-      <formula>$G41=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="120" priority="147">
-      <formula>$G41=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B41">
-    <cfRule type="expression" dxfId="119" priority="144">
-      <formula>$G41=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="118" priority="145">
-      <formula>$G41=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
-    <cfRule type="iconSet" priority="143">
+  <conditionalFormatting sqref="B9:I9">
+    <cfRule type="expression" dxfId="127" priority="137">
+      <formula>$G9=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="126" priority="138">
+      <formula>$G9=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="expression" dxfId="125" priority="135">
+      <formula>$G9=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="124" priority="136">
+      <formula>$G9=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="expression" dxfId="123" priority="133">
+      <formula>$G12=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="122" priority="134">
+      <formula>$G12=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="expression" dxfId="121" priority="131">
+      <formula>$G12=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="120" priority="132">
+      <formula>$G12=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:I8">
+    <cfRule type="expression" dxfId="119" priority="129">
+      <formula>$G8=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="130">
+      <formula>$G8=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="iconSet" priority="128">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4359,40 +4647,56 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="expression" dxfId="117" priority="139">
-      <formula>$G13=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="116" priority="140">
-      <formula>$G13=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15 A17:A24 A28">
-    <cfRule type="expression" dxfId="115" priority="137">
-      <formula>$G15=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="114" priority="138">
-      <formula>$G15=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="113" priority="135">
-      <formula>$G32=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="112" priority="136">
-      <formula>$G32=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="expression" dxfId="111" priority="126">
-      <formula>$G9=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="127">
-      <formula>$G9=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
-    <cfRule type="iconSet" priority="125">
+  <conditionalFormatting sqref="A7">
+    <cfRule type="expression" dxfId="117" priority="118">
+      <formula>$G7=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="119">
+      <formula>$G7=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="expression" dxfId="115" priority="124">
+      <formula>$G8=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="114" priority="125">
+      <formula>$G8=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="expression" dxfId="113" priority="122">
+      <formula>$G8=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="123">
+      <formula>$G8=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="expression" dxfId="111" priority="120">
+      <formula>$G7=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="121">
+      <formula>$G7=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="expression" dxfId="109" priority="111">
+      <formula>$G11=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="112">
+      <formula>$G11=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="expression" dxfId="107" priority="116">
+      <formula>$G11=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="117">
+      <formula>$G11=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="iconSet" priority="115">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4400,48 +4704,40 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:I9">
-    <cfRule type="expression" dxfId="109" priority="123">
-      <formula>$G9=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="108" priority="124">
-      <formula>$G9=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="expression" dxfId="107" priority="121">
-      <formula>$G9=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="122">
-      <formula>$G9=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="expression" dxfId="105" priority="119">
-      <formula>$G12=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="104" priority="120">
-      <formula>$G12=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="expression" dxfId="103" priority="117">
-      <formula>$G12=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="118">
-      <formula>$G12=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:I8">
-    <cfRule type="expression" dxfId="101" priority="115">
-      <formula>$G8=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="100" priority="116">
-      <formula>$G8=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
-    <cfRule type="iconSet" priority="114">
+  <conditionalFormatting sqref="B11:I11">
+    <cfRule type="expression" dxfId="105" priority="113">
+      <formula>$G11=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="114">
+      <formula>$G11=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="expression" dxfId="103" priority="104">
+      <formula>$G10=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="105">
+      <formula>$G10=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="expression" dxfId="101" priority="99">
+      <formula>$G16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="100">
+      <formula>$G16=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="expression" dxfId="99" priority="109">
+      <formula>$G10=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="110">
+      <formula>$G10=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="iconSet" priority="108">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4449,56 +4745,16 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="expression" dxfId="99" priority="104">
-      <formula>$G7=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="98" priority="105">
-      <formula>$G7=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="expression" dxfId="97" priority="110">
-      <formula>$G8=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="96" priority="111">
-      <formula>$G8=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="expression" dxfId="95" priority="108">
-      <formula>$G8=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="109">
-      <formula>$G8=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="expression" dxfId="93" priority="106">
-      <formula>$G7=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="92" priority="107">
-      <formula>$G7=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="expression" dxfId="91" priority="97">
-      <formula>$G11=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="90" priority="98">
-      <formula>$G11=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="expression" dxfId="89" priority="102">
-      <formula>$G11=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="88" priority="103">
-      <formula>$G11=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G11">
-    <cfRule type="iconSet" priority="101">
+  <conditionalFormatting sqref="B10:I10">
+    <cfRule type="expression" dxfId="97" priority="106">
+      <formula>$G10=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="107">
+      <formula>$G10=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
+    <cfRule type="iconSet" priority="103">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4506,40 +4762,16 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:I11">
-    <cfRule type="expression" dxfId="87" priority="99">
-      <formula>$G11=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="86" priority="100">
-      <formula>$G11=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="expression" dxfId="85" priority="90">
-      <formula>$G10=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="84" priority="91">
-      <formula>$G10=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="83" priority="85">
+  <conditionalFormatting sqref="B16:I16">
+    <cfRule type="expression" dxfId="95" priority="101">
       <formula>$G16=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="86">
+    <cfRule type="expression" dxfId="94" priority="102">
       <formula>$G16=2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="expression" dxfId="81" priority="95">
-      <formula>$G10=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="80" priority="96">
-      <formula>$G10=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
-    <cfRule type="iconSet" priority="94">
+  <conditionalFormatting sqref="G27">
+    <cfRule type="iconSet" priority="98">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4547,15 +4779,39 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10:I10">
-    <cfRule type="expression" dxfId="79" priority="92">
-      <formula>$G10=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="78" priority="93">
-      <formula>$G10=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G16">
+  <conditionalFormatting sqref="B27:I27">
+    <cfRule type="expression" dxfId="93" priority="96">
+      <formula>$G27=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="92" priority="97">
+      <formula>$G27=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="expression" dxfId="91" priority="94">
+      <formula>$G27=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="90" priority="95">
+      <formula>$G27=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34 C34:F34 H34:I34">
+    <cfRule type="expression" dxfId="89" priority="92">
+      <formula>$G34=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="93">
+      <formula>$G34=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="expression" dxfId="87" priority="90">
+      <formula>$G34=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="86" priority="91">
+      <formula>$G34=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34">
     <cfRule type="iconSet" priority="89">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -4564,16 +4820,32 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:I16">
-    <cfRule type="expression" dxfId="77" priority="87">
-      <formula>$G16=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="88">
-      <formula>$G16=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G27">
-    <cfRule type="iconSet" priority="84">
+  <conditionalFormatting sqref="G34">
+    <cfRule type="expression" dxfId="85" priority="87">
+      <formula>$G34=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="88">
+      <formula>$G34=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33 C33:F33 H33:I33">
+    <cfRule type="expression" dxfId="83" priority="85">
+      <formula>$G33=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="86">
+      <formula>$G33=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33">
+    <cfRule type="expression" dxfId="81" priority="83">
+      <formula>$G33=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="80" priority="84">
+      <formula>$G33=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G33">
+    <cfRule type="iconSet" priority="82">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4581,40 +4853,16 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27:I27">
-    <cfRule type="expression" dxfId="75" priority="82">
-      <formula>$G27=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="74" priority="83">
-      <formula>$G27=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="expression" dxfId="73" priority="80">
-      <formula>$G27=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="81">
-      <formula>$G27=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34 C34:F34 H34:I34">
-    <cfRule type="expression" dxfId="71" priority="78">
-      <formula>$G34=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="79">
-      <formula>$G34=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B34">
-    <cfRule type="expression" dxfId="69" priority="76">
-      <formula>$G34=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="68" priority="77">
-      <formula>$G34=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="iconSet" priority="75">
+  <conditionalFormatting sqref="G33">
+    <cfRule type="expression" dxfId="79" priority="80">
+      <formula>$G33=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="81">
+      <formula>$G33=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36">
+    <cfRule type="iconSet" priority="79">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4622,32 +4870,32 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="expression" dxfId="67" priority="73">
-      <formula>$G34=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="74">
-      <formula>$G34=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33 C33:F33 H33:I33">
-    <cfRule type="expression" dxfId="65" priority="71">
-      <formula>$G33=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="72">
-      <formula>$G33=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33">
-    <cfRule type="expression" dxfId="63" priority="69">
-      <formula>$G33=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="70">
-      <formula>$G33=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
-    <cfRule type="iconSet" priority="68">
+  <conditionalFormatting sqref="C36:I36">
+    <cfRule type="expression" dxfId="77" priority="77">
+      <formula>$G36=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="78">
+      <formula>$G36=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36">
+    <cfRule type="expression" dxfId="75" priority="75">
+      <formula>$G36=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="76">
+      <formula>$G36=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="expression" dxfId="73" priority="73">
+      <formula>$G36=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="74">
+      <formula>$G36=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G38">
+    <cfRule type="iconSet" priority="72">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4655,16 +4903,40 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
-    <cfRule type="expression" dxfId="61" priority="66">
-      <formula>$G33=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="60" priority="67">
-      <formula>$G33=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G36">
-    <cfRule type="iconSet" priority="65">
+  <conditionalFormatting sqref="C38:I38">
+    <cfRule type="expression" dxfId="71" priority="70">
+      <formula>$G38=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="71">
+      <formula>$G38=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38">
+    <cfRule type="expression" dxfId="69" priority="68">
+      <formula>$G38=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="69">
+      <formula>$G38=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="expression" dxfId="67" priority="66">
+      <formula>$G38=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="67">
+      <formula>$G38=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
+    <cfRule type="expression" dxfId="65" priority="64">
+      <formula>$G42=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="65">
+      <formula>$G42=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G42">
+    <cfRule type="iconSet" priority="63">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4672,32 +4944,32 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36:I36">
-    <cfRule type="expression" dxfId="59" priority="63">
-      <formula>$G36=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="64">
-      <formula>$G36=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
-    <cfRule type="expression" dxfId="57" priority="61">
-      <formula>$G36=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="62">
-      <formula>$G36=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="55" priority="59">
-      <formula>$G36=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="60">
-      <formula>$G36=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G38">
-    <cfRule type="iconSet" priority="58">
+  <conditionalFormatting sqref="C42:I42">
+    <cfRule type="expression" dxfId="63" priority="61">
+      <formula>$G42=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="62">
+      <formula>$G42=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42">
+    <cfRule type="expression" dxfId="61" priority="59">
+      <formula>$G42=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="60">
+      <formula>$G42=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
+    <cfRule type="expression" dxfId="59" priority="57">
+      <formula>$G43=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="58">
+      <formula>$G43=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43">
+    <cfRule type="iconSet" priority="56">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4705,39 +4977,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:I38">
-    <cfRule type="expression" dxfId="53" priority="56">
-      <formula>$G38=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="57">
-      <formula>$G38=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
-    <cfRule type="expression" dxfId="51" priority="54">
-      <formula>$G38=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="50" priority="55">
-      <formula>$G38=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
-    <cfRule type="expression" dxfId="49" priority="52">
-      <formula>$G38=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="53">
-      <formula>$G38=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="47" priority="50">
-      <formula>$G42=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="51">
-      <formula>$G42=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G42">
+  <conditionalFormatting sqref="C43:I43">
+    <cfRule type="expression" dxfId="57" priority="54">
+      <formula>$G43=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="55">
+      <formula>$G43=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43">
+    <cfRule type="expression" dxfId="55" priority="52">
+      <formula>$G43=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="53">
+      <formula>$G43=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44">
+    <cfRule type="expression" dxfId="53" priority="50">
+      <formula>$G44=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="51">
+      <formula>$G44=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G44">
     <cfRule type="iconSet" priority="49">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -4746,31 +5010,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42:I42">
-    <cfRule type="expression" dxfId="45" priority="47">
-      <formula>$G42=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="48">
-      <formula>$G42=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B42">
-    <cfRule type="expression" dxfId="43" priority="45">
-      <formula>$G42=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="46">
-      <formula>$G42=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43">
-    <cfRule type="expression" dxfId="41" priority="43">
-      <formula>$G43=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="44">
-      <formula>$G43=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G43">
+  <conditionalFormatting sqref="C44:I44">
+    <cfRule type="expression" dxfId="51" priority="47">
+      <formula>$G44=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="48">
+      <formula>$G44=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44">
+    <cfRule type="expression" dxfId="49" priority="45">
+      <formula>$G44=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="46">
+      <formula>$G44=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45">
+    <cfRule type="expression" dxfId="47" priority="43">
+      <formula>$G45=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="44">
+      <formula>$G45=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G45">
     <cfRule type="iconSet" priority="42">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -4779,31 +5043,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43:I43">
-    <cfRule type="expression" dxfId="39" priority="40">
-      <formula>$G43=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="41">
-      <formula>$G43=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B43">
-    <cfRule type="expression" dxfId="37" priority="38">
-      <formula>$G43=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="39">
-      <formula>$G43=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
-    <cfRule type="expression" dxfId="35" priority="36">
-      <formula>$G44=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="37">
-      <formula>$G44=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G44">
+  <conditionalFormatting sqref="C45:I45">
+    <cfRule type="expression" dxfId="45" priority="40">
+      <formula>$G45=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="41">
+      <formula>$G45=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
+    <cfRule type="expression" dxfId="43" priority="38">
+      <formula>$G45=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="39">
+      <formula>$G45=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46">
+    <cfRule type="expression" dxfId="41" priority="36">
+      <formula>$G46=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="37">
+      <formula>$G46=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G46">
     <cfRule type="iconSet" priority="35">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -4812,32 +5076,32 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C44:I44">
-    <cfRule type="expression" dxfId="33" priority="33">
-      <formula>$G44=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="34">
-      <formula>$G44=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B44">
-    <cfRule type="expression" dxfId="31" priority="31">
-      <formula>$G44=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="32">
-      <formula>$G44=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
-    <cfRule type="expression" dxfId="29" priority="29">
-      <formula>$G45=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="30">
-      <formula>$G45=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
-    <cfRule type="iconSet" priority="28">
+  <conditionalFormatting sqref="C46:I46">
+    <cfRule type="expression" dxfId="39" priority="33">
+      <formula>$G46=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="34">
+      <formula>$G46=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46">
+    <cfRule type="expression" dxfId="37" priority="31">
+      <formula>$G46=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="32">
+      <formula>$G46=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="expression" dxfId="35" priority="27">
+      <formula>$G47=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="28">
+      <formula>$G47=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G47">
+    <cfRule type="iconSet" priority="26">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4845,32 +5109,32 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45:I45">
-    <cfRule type="expression" dxfId="27" priority="26">
-      <formula>$G45=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="27">
-      <formula>$G45=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
-    <cfRule type="expression" dxfId="25" priority="24">
-      <formula>$G45=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="25">
-      <formula>$G45=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="23" priority="22">
-      <formula>$G46=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="23">
-      <formula>$G46=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G46">
-    <cfRule type="iconSet" priority="21">
+  <conditionalFormatting sqref="C47:I47">
+    <cfRule type="expression" dxfId="33" priority="24">
+      <formula>$G47=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="25">
+      <formula>$G47=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47">
+    <cfRule type="expression" dxfId="31" priority="22">
+      <formula>$G47=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="23">
+      <formula>$G47=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
+    <cfRule type="expression" dxfId="29" priority="20">
+      <formula>$G48=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="21">
+      <formula>$G48=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G48">
+    <cfRule type="iconSet" priority="19">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4878,31 +5142,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46:I46">
-    <cfRule type="expression" dxfId="21" priority="19">
-      <formula>$G46=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="20">
-      <formula>$G46=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="19" priority="17">
-      <formula>$G46=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="18">
-      <formula>$G46=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="17" priority="13">
-      <formula>$G47=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="14">
-      <formula>$G47=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G47">
+  <conditionalFormatting sqref="C48:I48">
+    <cfRule type="expression" dxfId="27" priority="17">
+      <formula>$G48=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="18">
+      <formula>$G48=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48">
+    <cfRule type="expression" dxfId="25" priority="15">
+      <formula>$G48=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="16">
+      <formula>$G48=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="expression" dxfId="23" priority="13">
+      <formula>$G49=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="14">
+      <formula>$G49=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G49">
     <cfRule type="iconSet" priority="12">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -4911,31 +5175,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47:I47">
-    <cfRule type="expression" dxfId="15" priority="10">
-      <formula>$G47=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="11">
-      <formula>$G47=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="13" priority="8">
-      <formula>$G47=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="9">
-      <formula>$G47=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
+  <conditionalFormatting sqref="C49:I49">
+    <cfRule type="expression" dxfId="19" priority="10">
+      <formula>$G49=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="11">
+      <formula>$G49=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49">
+    <cfRule type="expression" dxfId="15" priority="8">
+      <formula>$G49=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="9">
+      <formula>$G49=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
     <cfRule type="expression" dxfId="11" priority="6">
-      <formula>$G48=1</formula>
+      <formula>$G50=1</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="7">
-      <formula>$G48=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G48">
+      <formula>$G50=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G50">
     <cfRule type="iconSet" priority="5">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -4944,20 +5208,20 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48:I48">
+  <conditionalFormatting sqref="C50:I50">
     <cfRule type="expression" dxfId="7" priority="3">
-      <formula>$G48=1</formula>
+      <formula>$G50=1</formula>
     </cfRule>
     <cfRule type="expression" dxfId="6" priority="4">
-      <formula>$G48=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B48">
+      <formula>$G50=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50">
     <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$G48=1</formula>
+      <formula>$G50=1</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$G48=2</formula>
+      <formula>$G50=2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
NOVAS ALTERAÇÕES E FONTES COMPILADOS E AJUSTADOS 02/07/2013
</commit_message>
<xml_diff>
--- a/Acompanhamento de tarefas.xlsx
+++ b/Acompanhamento de tarefas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="179">
   <si>
     <t>Tarefas CCBA</t>
   </si>
@@ -541,6 +541,21 @@
   </si>
   <si>
     <t>PRÉ-PEDIDO DE VENDAS, ADICIONAR NOVAS REGRAS UTILIZANDO 6 TES PARA CONTAS ORDEM, ENTREGA FUTURAS, VENDA ADQUIRIDAS E VENDA PRODUTO PROPRIO - TODOS PARA FORA DO ESTADO. NO CASO DE CONTA ORDEM E ENTREGA FUTURA, ESTES DOIS CASOS IRÃO GERAR NOVOS PEDIDOS. ESSAS TES TERÁ UMA VERIFICAÇÃO QUE SERÁ: SE O PRODUTO B1_ORIGEM FIZER PARTE 1, 2 OU 3. SENDO INTERESTUAIS E ALIQUOTA DO ESTADO FOR IGUAL A 12%. COM TODAS ESSAS CONDIÇÕES SENDO VERDADEIRA, USARÁ A TES NOVA CORRESPONDENTE. SERÁ CRIADO PARAMETROS PARA USAR O "DE" - "PARA", PARA CRIAÇÃO DOS NOVOS PEDIDOS FEITO DE FORMA AUTOMATICA</t>
+  </si>
+  <si>
+    <t>ADICIONAR VALIDAÇÃO NA LINHA DO PEDIDO DE VENDA, QUE IRÁ VERIFICAR SE FOI INFORMADO UM DOS 4 TIPOS DE CFOP, SE ESTÁ USANDO ARMAZEM 30 E SE CONTROLA PORDER DE TERCEIRO. QUALQUER SITUAÇÃO DIFERENTE, DEVERÁ BLOQUEAR E APRESENTAR UMA INFORMAÇÃO</t>
+  </si>
+  <si>
+    <t>M410LIOK</t>
+  </si>
+  <si>
+    <t>EFETUAR AJUSTES DE VALIDAÇÃO PARA O PEDIDO DE VENDAS QUE NÃO ESTÁ VALIDANDO DE FORMA CORRETA, QUANDO É VENDA ORDEM, VENDA ENTREGA FUTURA E NORMAL</t>
+  </si>
+  <si>
+    <t>CCRFAT05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRIAR UM CONTROLE DE LOG PARA CADASTRO DE CLIENTES, DETALHANDO COM USUÁRIO QUE FEZ A ALTERAÇÃO, DATA E HORA, AÇÃO QUE FOI TOMADA </t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1217,259 @@
     <cellStyle name="Título" xfId="1" builtinId="15"/>
     <cellStyle name="Total" xfId="5" builtinId="25"/>
   </cellStyles>
-  <dxfs count="198">
+  <dxfs count="234">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2895,11 +3162,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan1"/>
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
+      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2944,7 +3211,7 @@
       </c>
       <c r="J2" s="78">
         <f>COUNTIF(G6:G112,2)</f>
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2963,7 +3230,7 @@
       </c>
       <c r="J3" s="79">
         <f>COUNTIF(G6:G112,1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4042,7 +4309,7 @@
     </row>
     <row r="41" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A41" s="65">
-        <f t="shared" ref="A41:A55" si="4">A40+1</f>
+        <f t="shared" ref="A41:A58" si="4">A40+1</f>
         <v>34</v>
       </c>
       <c r="B41" s="73" t="s">
@@ -4487,6 +4754,92 @@
         <v>41453</v>
       </c>
       <c r="I55" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="65">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="B56" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="C56" s="67">
+        <v>41456</v>
+      </c>
+      <c r="D56" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="E56" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="F56" s="72" t="s">
+        <v>175</v>
+      </c>
+      <c r="G56" s="69">
+        <v>2</v>
+      </c>
+      <c r="H56" s="70">
+        <v>41456</v>
+      </c>
+      <c r="I56" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A57" s="65">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="B57" s="73" t="s">
+        <v>176</v>
+      </c>
+      <c r="C57" s="67">
+        <v>41456</v>
+      </c>
+      <c r="D57" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="E57" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="F57" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="G57" s="69">
+        <v>2</v>
+      </c>
+      <c r="H57" s="70">
+        <v>41456</v>
+      </c>
+      <c r="I57" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A58" s="65">
+        <f t="shared" si="4"/>
+        <v>51</v>
+      </c>
+      <c r="B58" s="73" t="s">
+        <v>178</v>
+      </c>
+      <c r="C58" s="67">
+        <v>41456</v>
+      </c>
+      <c r="D58" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="E58" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="F58" s="72"/>
+      <c r="G58" s="69">
+        <v>1</v>
+      </c>
+      <c r="H58" s="70"/>
+      <c r="I58" s="71">
         <v>0</v>
       </c>
     </row>
@@ -4496,7 +4849,7 @@
     <mergeCell ref="B2:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="H2">
-    <cfRule type="iconSet" priority="274">
+    <cfRule type="iconSet" priority="295">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4505,6 +4858,109 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
+    <cfRule type="iconSet" priority="294">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="1" gte="0"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="iconSet" priority="293">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="1" gte="0"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="iconSet" priority="291">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="1" gte="0"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:I6 B7:I7 A25:I26 A39:A41 A37:I37">
+    <cfRule type="expression" dxfId="233" priority="289">
+      <formula>$G6=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="232" priority="290">
+      <formula>$G6=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="iconSet" priority="288">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="1" gte="0"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:I12">
+    <cfRule type="expression" dxfId="231" priority="286">
+      <formula>$G12=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="230" priority="287">
+      <formula>$G12=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13">
+    <cfRule type="iconSet" priority="285">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="1" gte="0"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:I13">
+    <cfRule type="expression" dxfId="229" priority="283">
+      <formula>$G13=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="228" priority="284">
+      <formula>$G13=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="iconSet" priority="282">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="1" gte="0"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:I14">
+    <cfRule type="expression" dxfId="227" priority="280">
+      <formula>$G14=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="226" priority="281">
+      <formula>$G14=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15">
+    <cfRule type="iconSet" priority="276">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="1" gte="0"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:I15">
+    <cfRule type="expression" dxfId="225" priority="274">
+      <formula>$G15=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="224" priority="275">
+      <formula>$G15=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17">
     <cfRule type="iconSet" priority="273">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -4513,33 +4969,15 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="iconSet" priority="272">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="1" gte="0"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="iconSet" priority="270">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="1" gte="0"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A6:I6 B7:I7 A25:I26 A39:A41 A37:I37">
-    <cfRule type="expression" dxfId="197" priority="268">
-      <formula>$G6=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="196" priority="269">
-      <formula>$G6=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12">
+  <conditionalFormatting sqref="B17:I17">
+    <cfRule type="expression" dxfId="223" priority="271">
+      <formula>$G17=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="222" priority="272">
+      <formula>$G17=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G19:G22">
     <cfRule type="iconSet" priority="267">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -4548,15 +4986,15 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:I12">
-    <cfRule type="expression" dxfId="195" priority="265">
-      <formula>$G12=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="194" priority="266">
-      <formula>$G12=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G13">
+  <conditionalFormatting sqref="B19:I22">
+    <cfRule type="expression" dxfId="221" priority="265">
+      <formula>$G19=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="220" priority="266">
+      <formula>$G19=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
     <cfRule type="iconSet" priority="264">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -4565,15 +5003,15 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:I13">
-    <cfRule type="expression" dxfId="193" priority="262">
-      <formula>$G13=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="192" priority="263">
-      <formula>$G13=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G14">
+  <conditionalFormatting sqref="B18:I18">
+    <cfRule type="expression" dxfId="219" priority="262">
+      <formula>$G18=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="218" priority="263">
+      <formula>$G18=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28 G23:G26">
     <cfRule type="iconSet" priority="261">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -4582,15 +5020,32 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:I14">
-    <cfRule type="expression" dxfId="191" priority="259">
-      <formula>$G14=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="190" priority="260">
-      <formula>$G14=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G15">
+  <conditionalFormatting sqref="B23:I24 B28:I28">
+    <cfRule type="expression" dxfId="217" priority="259">
+      <formula>$G23=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="216" priority="260">
+      <formula>$G23=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G29:G30">
+    <cfRule type="iconSet" priority="258">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="1" gte="0"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:I30">
+    <cfRule type="expression" dxfId="215" priority="256">
+      <formula>$G29=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="214" priority="257">
+      <formula>$G29=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G31">
     <cfRule type="iconSet" priority="255">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -4599,15 +5054,15 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:I15">
-    <cfRule type="expression" dxfId="189" priority="253">
-      <formula>$G15=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="188" priority="254">
-      <formula>$G15=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G17">
+  <conditionalFormatting sqref="A31:I31">
+    <cfRule type="expression" dxfId="213" priority="253">
+      <formula>$G31=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="212" priority="254">
+      <formula>$G31=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G32">
     <cfRule type="iconSet" priority="252">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -4616,16 +5071,40 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:I17">
-    <cfRule type="expression" dxfId="187" priority="250">
-      <formula>$G17=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="186" priority="251">
-      <formula>$G17=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G19:G22">
-    <cfRule type="iconSet" priority="246">
+  <conditionalFormatting sqref="C32:I32">
+    <cfRule type="expression" dxfId="211" priority="250">
+      <formula>$G32=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="210" priority="251">
+      <formula>$G32=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="expression" dxfId="209" priority="248">
+      <formula>$G32=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="208" priority="249">
+      <formula>$G32=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35 C35:F35 H35:I35">
+    <cfRule type="expression" dxfId="207" priority="245">
+      <formula>$G35=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="206" priority="246">
+      <formula>$G35=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="expression" dxfId="205" priority="243">
+      <formula>$G35=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="204" priority="244">
+      <formula>$G35=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="iconSet" priority="242">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4633,16 +5112,16 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:I22">
-    <cfRule type="expression" dxfId="185" priority="244">
-      <formula>$G19=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="184" priority="245">
-      <formula>$G19=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G18">
-    <cfRule type="iconSet" priority="243">
+  <conditionalFormatting sqref="G35">
+    <cfRule type="expression" dxfId="203" priority="240">
+      <formula>$G35=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="202" priority="241">
+      <formula>$G35=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G39">
+    <cfRule type="iconSet" priority="238">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4650,16 +5129,24 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:I18">
-    <cfRule type="expression" dxfId="183" priority="241">
-      <formula>$G18=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="182" priority="242">
-      <formula>$G18=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G28 G23:G26">
-    <cfRule type="iconSet" priority="240">
+  <conditionalFormatting sqref="C39:I39">
+    <cfRule type="expression" dxfId="201" priority="236">
+      <formula>$G39=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="200" priority="237">
+      <formula>$G39=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39">
+    <cfRule type="expression" dxfId="199" priority="234">
+      <formula>$G39=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="198" priority="235">
+      <formula>$G39=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G37">
+    <cfRule type="iconSet" priority="228">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4667,16 +5154,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23:I24 B28:I28">
-    <cfRule type="expression" dxfId="181" priority="238">
-      <formula>$G23=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="180" priority="239">
-      <formula>$G23=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G29:G30">
-    <cfRule type="iconSet" priority="237">
+  <conditionalFormatting sqref="G40">
+    <cfRule type="iconSet" priority="223">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4684,16 +5163,24 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A29:I30">
-    <cfRule type="expression" dxfId="179" priority="235">
-      <formula>$G29=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="178" priority="236">
-      <formula>$G29=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G31">
-    <cfRule type="iconSet" priority="234">
+  <conditionalFormatting sqref="C40:I40">
+    <cfRule type="expression" dxfId="197" priority="221">
+      <formula>$G40=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="196" priority="222">
+      <formula>$G40=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="expression" dxfId="195" priority="219">
+      <formula>$G40=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="194" priority="220">
+      <formula>$G40=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="iconSet" priority="218">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4701,16 +5188,24 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A31:I31">
-    <cfRule type="expression" dxfId="177" priority="232">
-      <formula>$G31=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="176" priority="233">
-      <formula>$G31=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G32">
-    <cfRule type="iconSet" priority="231">
+  <conditionalFormatting sqref="C41:I41">
+    <cfRule type="expression" dxfId="193" priority="216">
+      <formula>$G41=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="192" priority="217">
+      <formula>$G41=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="expression" dxfId="191" priority="214">
+      <formula>$G41=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="190" priority="215">
+      <formula>$G41=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="iconSet" priority="213">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4718,40 +5213,40 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32:I32">
-    <cfRule type="expression" dxfId="175" priority="229">
+  <conditionalFormatting sqref="A13">
+    <cfRule type="expression" dxfId="189" priority="209">
+      <formula>$G13=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="188" priority="210">
+      <formula>$G13=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15 A17:A24 A28">
+    <cfRule type="expression" dxfId="187" priority="207">
+      <formula>$G15=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="186" priority="208">
+      <formula>$G15=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="expression" dxfId="185" priority="205">
       <formula>$G32=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="230">
+    <cfRule type="expression" dxfId="184" priority="206">
       <formula>$G32=2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="173" priority="227">
-      <formula>$G32=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="172" priority="228">
-      <formula>$G32=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35 C35:F35 H35:I35">
-    <cfRule type="expression" dxfId="171" priority="224">
-      <formula>$G35=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="170" priority="225">
-      <formula>$G35=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B35">
-    <cfRule type="expression" dxfId="169" priority="222">
-      <formula>$G35=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="168" priority="223">
-      <formula>$G35=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="iconSet" priority="221">
+  <conditionalFormatting sqref="A9">
+    <cfRule type="expression" dxfId="183" priority="196">
+      <formula>$G9=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="182" priority="197">
+      <formula>$G9=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="iconSet" priority="195">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4759,16 +5254,48 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="expression" dxfId="167" priority="219">
-      <formula>$G35=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="166" priority="220">
-      <formula>$G35=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G39">
-    <cfRule type="iconSet" priority="217">
+  <conditionalFormatting sqref="B9:I9">
+    <cfRule type="expression" dxfId="181" priority="193">
+      <formula>$G9=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="180" priority="194">
+      <formula>$G9=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="expression" dxfId="179" priority="191">
+      <formula>$G9=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="178" priority="192">
+      <formula>$G9=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="expression" dxfId="177" priority="189">
+      <formula>$G12=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="176" priority="190">
+      <formula>$G12=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="expression" dxfId="175" priority="187">
+      <formula>$G12=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="174" priority="188">
+      <formula>$G12=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:I8">
+    <cfRule type="expression" dxfId="173" priority="185">
+      <formula>$G8=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="172" priority="186">
+      <formula>$G8=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="iconSet" priority="184">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4776,24 +5303,56 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39:I39">
-    <cfRule type="expression" dxfId="165" priority="215">
-      <formula>$G39=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="164" priority="216">
-      <formula>$G39=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
-    <cfRule type="expression" dxfId="163" priority="213">
-      <formula>$G39=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="162" priority="214">
-      <formula>$G39=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G37">
-    <cfRule type="iconSet" priority="207">
+  <conditionalFormatting sqref="A7">
+    <cfRule type="expression" dxfId="171" priority="174">
+      <formula>$G7=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="170" priority="175">
+      <formula>$G7=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="expression" dxfId="169" priority="180">
+      <formula>$G8=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="168" priority="181">
+      <formula>$G8=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="expression" dxfId="167" priority="178">
+      <formula>$G8=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="166" priority="179">
+      <formula>$G8=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="expression" dxfId="165" priority="176">
+      <formula>$G7=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="164" priority="177">
+      <formula>$G7=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="expression" dxfId="163" priority="167">
+      <formula>$G11=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="162" priority="168">
+      <formula>$G11=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="expression" dxfId="161" priority="172">
+      <formula>$G11=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="160" priority="173">
+      <formula>$G11=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="iconSet" priority="171">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4801,8 +5360,40 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
-    <cfRule type="iconSet" priority="202">
+  <conditionalFormatting sqref="B11:I11">
+    <cfRule type="expression" dxfId="159" priority="169">
+      <formula>$G11=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="158" priority="170">
+      <formula>$G11=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="expression" dxfId="157" priority="160">
+      <formula>$G10=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="156" priority="161">
+      <formula>$G10=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="expression" dxfId="155" priority="155">
+      <formula>$G16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="154" priority="156">
+      <formula>$G16=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="expression" dxfId="153" priority="165">
+      <formula>$G10=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="152" priority="166">
+      <formula>$G10=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="iconSet" priority="164">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4810,24 +5401,16 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40:I40">
-    <cfRule type="expression" dxfId="161" priority="200">
-      <formula>$G40=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="160" priority="201">
-      <formula>$G40=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="159" priority="198">
-      <formula>$G40=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="158" priority="199">
-      <formula>$G40=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G41">
-    <cfRule type="iconSet" priority="197">
+  <conditionalFormatting sqref="B10:I10">
+    <cfRule type="expression" dxfId="151" priority="162">
+      <formula>$G10=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="150" priority="163">
+      <formula>$G10=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
+    <cfRule type="iconSet" priority="159">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4835,24 +5418,16 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41:I41">
-    <cfRule type="expression" dxfId="157" priority="195">
-      <formula>$G41=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="156" priority="196">
-      <formula>$G41=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B41">
-    <cfRule type="expression" dxfId="155" priority="193">
-      <formula>$G41=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="154" priority="194">
-      <formula>$G41=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
-    <cfRule type="iconSet" priority="192">
+  <conditionalFormatting sqref="B16:I16">
+    <cfRule type="expression" dxfId="149" priority="157">
+      <formula>$G16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="148" priority="158">
+      <formula>$G16=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27">
+    <cfRule type="iconSet" priority="154">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4860,40 +5435,40 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="expression" dxfId="153" priority="188">
-      <formula>$G13=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="152" priority="189">
-      <formula>$G13=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15 A17:A24 A28">
-    <cfRule type="expression" dxfId="151" priority="186">
-      <formula>$G15=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="150" priority="187">
-      <formula>$G15=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="149" priority="184">
-      <formula>$G32=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="148" priority="185">
-      <formula>$G32=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="expression" dxfId="147" priority="175">
-      <formula>$G9=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="146" priority="176">
-      <formula>$G9=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
-    <cfRule type="iconSet" priority="174">
+  <conditionalFormatting sqref="B27:I27">
+    <cfRule type="expression" dxfId="147" priority="152">
+      <formula>$G27=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="146" priority="153">
+      <formula>$G27=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="expression" dxfId="145" priority="150">
+      <formula>$G27=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="151">
+      <formula>$G27=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34 C34:F34 H34:I34">
+    <cfRule type="expression" dxfId="143" priority="148">
+      <formula>$G34=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="142" priority="149">
+      <formula>$G34=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="expression" dxfId="141" priority="146">
+      <formula>$G34=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="147">
+      <formula>$G34=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34">
+    <cfRule type="iconSet" priority="145">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4901,162 +5476,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:I9">
-    <cfRule type="expression" dxfId="145" priority="172">
-      <formula>$G9=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="144" priority="173">
-      <formula>$G9=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="expression" dxfId="143" priority="170">
-      <formula>$G9=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="142" priority="171">
-      <formula>$G9=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="expression" dxfId="141" priority="168">
-      <formula>$G12=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="140" priority="169">
-      <formula>$G12=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="expression" dxfId="139" priority="166">
-      <formula>$G12=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="138" priority="167">
-      <formula>$G12=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:I8">
-    <cfRule type="expression" dxfId="137" priority="164">
-      <formula>$G8=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="136" priority="165">
-      <formula>$G8=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
-    <cfRule type="iconSet" priority="163">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="1" gte="0"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="expression" dxfId="135" priority="153">
-      <formula>$G7=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="134" priority="154">
-      <formula>$G7=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="expression" dxfId="133" priority="159">
-      <formula>$G8=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="132" priority="160">
-      <formula>$G8=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="expression" dxfId="131" priority="157">
-      <formula>$G8=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="130" priority="158">
-      <formula>$G8=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="expression" dxfId="129" priority="155">
-      <formula>$G7=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="128" priority="156">
-      <formula>$G7=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="expression" dxfId="127" priority="146">
-      <formula>$G11=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="126" priority="147">
-      <formula>$G11=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="expression" dxfId="125" priority="151">
-      <formula>$G11=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="124" priority="152">
-      <formula>$G11=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G11">
-    <cfRule type="iconSet" priority="150">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="1" gte="0"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11:I11">
-    <cfRule type="expression" dxfId="123" priority="148">
-      <formula>$G11=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="122" priority="149">
-      <formula>$G11=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="expression" dxfId="121" priority="139">
-      <formula>$G10=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="120" priority="140">
-      <formula>$G10=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="119" priority="134">
-      <formula>$G16=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="118" priority="135">
-      <formula>$G16=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="expression" dxfId="117" priority="144">
-      <formula>$G10=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="116" priority="145">
-      <formula>$G10=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
-    <cfRule type="iconSet" priority="143">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="1" gte="0"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B10:I10">
-    <cfRule type="expression" dxfId="115" priority="141">
-      <formula>$G10=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="114" priority="142">
-      <formula>$G10=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G16">
+  <conditionalFormatting sqref="G34">
+    <cfRule type="expression" dxfId="139" priority="143">
+      <formula>$G34=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="138" priority="144">
+      <formula>$G34=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33 C33:F33 H33:I33">
+    <cfRule type="expression" dxfId="137" priority="141">
+      <formula>$G33=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="136" priority="142">
+      <formula>$G33=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33">
+    <cfRule type="expression" dxfId="135" priority="139">
+      <formula>$G33=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="134" priority="140">
+      <formula>$G33=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G33">
     <cfRule type="iconSet" priority="138">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5065,16 +5509,16 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:I16">
-    <cfRule type="expression" dxfId="113" priority="136">
-      <formula>$G16=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="112" priority="137">
-      <formula>$G16=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G27">
-    <cfRule type="iconSet" priority="133">
+  <conditionalFormatting sqref="G33">
+    <cfRule type="expression" dxfId="133" priority="136">
+      <formula>$G33=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="132" priority="137">
+      <formula>$G33=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36">
+    <cfRule type="iconSet" priority="135">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5082,40 +5526,32 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27:I27">
-    <cfRule type="expression" dxfId="111" priority="131">
-      <formula>$G27=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="132">
-      <formula>$G27=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="expression" dxfId="109" priority="129">
-      <formula>$G27=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="108" priority="130">
-      <formula>$G27=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34 C34:F34 H34:I34">
-    <cfRule type="expression" dxfId="107" priority="127">
-      <formula>$G34=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="128">
-      <formula>$G34=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B34">
-    <cfRule type="expression" dxfId="105" priority="125">
-      <formula>$G34=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="104" priority="126">
-      <formula>$G34=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="iconSet" priority="124">
+  <conditionalFormatting sqref="C36:I36">
+    <cfRule type="expression" dxfId="131" priority="133">
+      <formula>$G36=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="130" priority="134">
+      <formula>$G36=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36">
+    <cfRule type="expression" dxfId="129" priority="131">
+      <formula>$G36=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="128" priority="132">
+      <formula>$G36=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="expression" dxfId="127" priority="129">
+      <formula>$G36=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="126" priority="130">
+      <formula>$G36=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G38">
+    <cfRule type="iconSet" priority="128">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5123,32 +5559,40 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="expression" dxfId="103" priority="122">
-      <formula>$G34=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="123">
-      <formula>$G34=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33 C33:F33 H33:I33">
-    <cfRule type="expression" dxfId="101" priority="120">
-      <formula>$G33=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="100" priority="121">
-      <formula>$G33=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33">
-    <cfRule type="expression" dxfId="99" priority="118">
-      <formula>$G33=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="98" priority="119">
-      <formula>$G33=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
-    <cfRule type="iconSet" priority="117">
+  <conditionalFormatting sqref="C38:I38">
+    <cfRule type="expression" dxfId="125" priority="126">
+      <formula>$G38=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="124" priority="127">
+      <formula>$G38=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38">
+    <cfRule type="expression" dxfId="123" priority="124">
+      <formula>$G38=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="122" priority="125">
+      <formula>$G38=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="expression" dxfId="121" priority="122">
+      <formula>$G38=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="120" priority="123">
+      <formula>$G38=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
+    <cfRule type="expression" dxfId="119" priority="120">
+      <formula>$G42=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="121">
+      <formula>$G42=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G42">
+    <cfRule type="iconSet" priority="119">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5156,16 +5600,32 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
-    <cfRule type="expression" dxfId="97" priority="115">
-      <formula>$G33=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="96" priority="116">
-      <formula>$G33=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G36">
-    <cfRule type="iconSet" priority="114">
+  <conditionalFormatting sqref="C42:I42">
+    <cfRule type="expression" dxfId="117" priority="117">
+      <formula>$G42=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="118">
+      <formula>$G42=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42">
+    <cfRule type="expression" dxfId="115" priority="115">
+      <formula>$G42=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="114" priority="116">
+      <formula>$G42=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
+    <cfRule type="expression" dxfId="113" priority="113">
+      <formula>$G43=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="114">
+      <formula>$G43=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43">
+    <cfRule type="iconSet" priority="112">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5173,32 +5633,32 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36:I36">
-    <cfRule type="expression" dxfId="95" priority="112">
-      <formula>$G36=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="113">
-      <formula>$G36=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
-    <cfRule type="expression" dxfId="93" priority="110">
-      <formula>$G36=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="92" priority="111">
-      <formula>$G36=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="91" priority="108">
-      <formula>$G36=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="90" priority="109">
-      <formula>$G36=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G38">
-    <cfRule type="iconSet" priority="107">
+  <conditionalFormatting sqref="C43:I43">
+    <cfRule type="expression" dxfId="111" priority="110">
+      <formula>$G43=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="111">
+      <formula>$G43=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43">
+    <cfRule type="expression" dxfId="109" priority="108">
+      <formula>$G43=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="109">
+      <formula>$G43=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44">
+    <cfRule type="expression" dxfId="107" priority="106">
+      <formula>$G44=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="107">
+      <formula>$G44=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G44">
+    <cfRule type="iconSet" priority="105">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5206,39 +5666,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:I38">
-    <cfRule type="expression" dxfId="89" priority="105">
-      <formula>$G38=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="88" priority="106">
-      <formula>$G38=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
-    <cfRule type="expression" dxfId="87" priority="103">
-      <formula>$G38=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="86" priority="104">
-      <formula>$G38=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
-    <cfRule type="expression" dxfId="85" priority="101">
-      <formula>$G38=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="84" priority="102">
-      <formula>$G38=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="83" priority="99">
-      <formula>$G42=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="100">
-      <formula>$G42=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G42">
+  <conditionalFormatting sqref="C44:I44">
+    <cfRule type="expression" dxfId="105" priority="103">
+      <formula>$G44=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="104">
+      <formula>$G44=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44">
+    <cfRule type="expression" dxfId="103" priority="101">
+      <formula>$G44=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="102">
+      <formula>$G44=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45">
+    <cfRule type="expression" dxfId="101" priority="99">
+      <formula>$G45=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="100">
+      <formula>$G45=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G45">
     <cfRule type="iconSet" priority="98">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5247,31 +5699,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42:I42">
-    <cfRule type="expression" dxfId="81" priority="96">
-      <formula>$G42=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="80" priority="97">
-      <formula>$G42=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B42">
-    <cfRule type="expression" dxfId="79" priority="94">
-      <formula>$G42=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="78" priority="95">
-      <formula>$G42=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43">
-    <cfRule type="expression" dxfId="77" priority="92">
-      <formula>$G43=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="93">
-      <formula>$G43=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G43">
+  <conditionalFormatting sqref="C45:I45">
+    <cfRule type="expression" dxfId="99" priority="96">
+      <formula>$G45=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="97">
+      <formula>$G45=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
+    <cfRule type="expression" dxfId="97" priority="94">
+      <formula>$G45=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="95">
+      <formula>$G45=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46">
+    <cfRule type="expression" dxfId="95" priority="92">
+      <formula>$G46=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="94" priority="93">
+      <formula>$G46=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G46">
     <cfRule type="iconSet" priority="91">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5280,32 +5732,32 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43:I43">
-    <cfRule type="expression" dxfId="75" priority="89">
-      <formula>$G43=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="74" priority="90">
-      <formula>$G43=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B43">
-    <cfRule type="expression" dxfId="73" priority="87">
-      <formula>$G43=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="88">
-      <formula>$G43=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
-    <cfRule type="expression" dxfId="71" priority="85">
-      <formula>$G44=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="86">
-      <formula>$G44=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G44">
-    <cfRule type="iconSet" priority="84">
+  <conditionalFormatting sqref="C46:I46">
+    <cfRule type="expression" dxfId="93" priority="89">
+      <formula>$G46=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="92" priority="90">
+      <formula>$G46=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46">
+    <cfRule type="expression" dxfId="91" priority="87">
+      <formula>$G46=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="90" priority="88">
+      <formula>$G46=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="expression" dxfId="89" priority="83">
+      <formula>$G47=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="84">
+      <formula>$G47=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G47">
+    <cfRule type="iconSet" priority="82">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5313,32 +5765,32 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C44:I44">
-    <cfRule type="expression" dxfId="69" priority="82">
-      <formula>$G44=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="68" priority="83">
-      <formula>$G44=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B44">
-    <cfRule type="expression" dxfId="67" priority="80">
-      <formula>$G44=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="81">
-      <formula>$G44=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
-    <cfRule type="expression" dxfId="65" priority="78">
-      <formula>$G45=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="79">
-      <formula>$G45=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
-    <cfRule type="iconSet" priority="77">
+  <conditionalFormatting sqref="C47:I47">
+    <cfRule type="expression" dxfId="87" priority="80">
+      <formula>$G47=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="86" priority="81">
+      <formula>$G47=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47">
+    <cfRule type="expression" dxfId="85" priority="78">
+      <formula>$G47=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="79">
+      <formula>$G47=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
+    <cfRule type="expression" dxfId="83" priority="76">
+      <formula>$G48=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="77">
+      <formula>$G48=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G48">
+    <cfRule type="iconSet" priority="75">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5346,32 +5798,32 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45:I45">
-    <cfRule type="expression" dxfId="63" priority="75">
-      <formula>$G45=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="76">
-      <formula>$G45=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
-    <cfRule type="expression" dxfId="61" priority="73">
-      <formula>$G45=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="60" priority="74">
-      <formula>$G45=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="59" priority="71">
-      <formula>$G46=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="72">
-      <formula>$G46=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G46">
-    <cfRule type="iconSet" priority="70">
+  <conditionalFormatting sqref="C48:I48">
+    <cfRule type="expression" dxfId="81" priority="73">
+      <formula>$G48=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="80" priority="74">
+      <formula>$G48=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48">
+    <cfRule type="expression" dxfId="79" priority="71">
+      <formula>$G48=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="72">
+      <formula>$G48=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="expression" dxfId="77" priority="69">
+      <formula>$G49=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="70">
+      <formula>$G49=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G49">
+    <cfRule type="iconSet" priority="68">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5379,31 +5831,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46:I46">
-    <cfRule type="expression" dxfId="57" priority="68">
-      <formula>$G46=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="69">
-      <formula>$G46=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="55" priority="66">
-      <formula>$G46=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="67">
-      <formula>$G46=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="53" priority="62">
-      <formula>$G47=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="63">
-      <formula>$G47=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G47">
+  <conditionalFormatting sqref="C49:I49">
+    <cfRule type="expression" dxfId="75" priority="66">
+      <formula>$G49=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="67">
+      <formula>$G49=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49">
+    <cfRule type="expression" dxfId="73" priority="64">
+      <formula>$G49=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="65">
+      <formula>$G49=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="expression" dxfId="71" priority="62">
+      <formula>$G50=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="63">
+      <formula>$G50=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G50">
     <cfRule type="iconSet" priority="61">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5412,31 +5864,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47:I47">
-    <cfRule type="expression" dxfId="51" priority="59">
-      <formula>$G47=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="50" priority="60">
-      <formula>$G47=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="49" priority="57">
-      <formula>$G47=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="58">
-      <formula>$G47=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
-    <cfRule type="expression" dxfId="47" priority="55">
-      <formula>$G48=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="56">
-      <formula>$G48=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G48">
+  <conditionalFormatting sqref="C50:I50">
+    <cfRule type="expression" dxfId="69" priority="59">
+      <formula>$G50=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="60">
+      <formula>$G50=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50">
+    <cfRule type="expression" dxfId="67" priority="57">
+      <formula>$G50=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="58">
+      <formula>$G50=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="expression" dxfId="65" priority="55">
+      <formula>$G51=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="56">
+      <formula>$G51=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G51">
     <cfRule type="iconSet" priority="54">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5445,31 +5897,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48:I48">
-    <cfRule type="expression" dxfId="45" priority="52">
-      <formula>$G48=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="53">
-      <formula>$G48=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="43" priority="50">
-      <formula>$G48=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="51">
-      <formula>$G48=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="expression" dxfId="41" priority="48">
-      <formula>$G49=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="49">
-      <formula>$G49=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G49">
+  <conditionalFormatting sqref="C51:I51">
+    <cfRule type="expression" dxfId="63" priority="52">
+      <formula>$G51=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="53">
+      <formula>$G51=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B51">
+    <cfRule type="expression" dxfId="61" priority="50">
+      <formula>$G51=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="51">
+      <formula>$G51=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="expression" dxfId="59" priority="48">
+      <formula>$G52=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="49">
+      <formula>$G52=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G52">
     <cfRule type="iconSet" priority="47">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5478,31 +5930,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:I49">
-    <cfRule type="expression" dxfId="39" priority="45">
-      <formula>$G49=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="46">
-      <formula>$G49=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49">
-    <cfRule type="expression" dxfId="37" priority="43">
-      <formula>$G49=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="44">
-      <formula>$G49=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50">
-    <cfRule type="expression" dxfId="35" priority="41">
-      <formula>$G50=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="42">
-      <formula>$G50=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G50">
+  <conditionalFormatting sqref="C52:I52">
+    <cfRule type="expression" dxfId="57" priority="45">
+      <formula>$G52=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="46">
+      <formula>$G52=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52">
+    <cfRule type="expression" dxfId="55" priority="43">
+      <formula>$G52=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="44">
+      <formula>$G52=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A53">
+    <cfRule type="expression" dxfId="53" priority="41">
+      <formula>$G53=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="42">
+      <formula>$G53=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G53">
     <cfRule type="iconSet" priority="40">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5511,31 +5963,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50:I50">
-    <cfRule type="expression" dxfId="33" priority="38">
-      <formula>$G50=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="39">
-      <formula>$G50=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B50">
-    <cfRule type="expression" dxfId="31" priority="36">
-      <formula>$G50=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="37">
-      <formula>$G50=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
-    <cfRule type="expression" dxfId="29" priority="34">
-      <formula>$G51=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="35">
-      <formula>$G51=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G51">
+  <conditionalFormatting sqref="C53:I53">
+    <cfRule type="expression" dxfId="51" priority="38">
+      <formula>$G53=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="39">
+      <formula>$G53=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53">
+    <cfRule type="expression" dxfId="49" priority="36">
+      <formula>$G53=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="37">
+      <formula>$G53=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54">
+    <cfRule type="expression" dxfId="47" priority="34">
+      <formula>$G54=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="35">
+      <formula>$G54=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G54">
     <cfRule type="iconSet" priority="33">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5544,31 +5996,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C51:I51">
-    <cfRule type="expression" dxfId="27" priority="31">
-      <formula>$G51=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="32">
-      <formula>$G51=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B51">
-    <cfRule type="expression" dxfId="25" priority="29">
-      <formula>$G51=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="30">
-      <formula>$G51=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52">
-    <cfRule type="expression" dxfId="23" priority="27">
-      <formula>$G52=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="28">
-      <formula>$G52=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G52">
+  <conditionalFormatting sqref="C54:I54">
+    <cfRule type="expression" dxfId="45" priority="31">
+      <formula>$G54=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="32">
+      <formula>$G54=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54">
+    <cfRule type="expression" dxfId="43" priority="29">
+      <formula>$G54=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="30">
+      <formula>$G54=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="expression" dxfId="41" priority="27">
+      <formula>$G55=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="28">
+      <formula>$G55=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G55">
     <cfRule type="iconSet" priority="26">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5577,31 +6029,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52:I52">
-    <cfRule type="expression" dxfId="21" priority="24">
-      <formula>$G52=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="25">
-      <formula>$G52=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B52">
-    <cfRule type="expression" dxfId="19" priority="22">
-      <formula>$G52=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="23">
-      <formula>$G52=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
-    <cfRule type="expression" dxfId="17" priority="20">
-      <formula>$G53=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="21">
-      <formula>$G53=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G53">
+  <conditionalFormatting sqref="C55:I55">
+    <cfRule type="expression" dxfId="39" priority="24">
+      <formula>$G55=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="25">
+      <formula>$G55=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B55">
+    <cfRule type="expression" dxfId="37" priority="22">
+      <formula>$G55=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="23">
+      <formula>$G55=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56">
+    <cfRule type="expression" dxfId="35" priority="20">
+      <formula>$G56=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="21">
+      <formula>$G56=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G56">
     <cfRule type="iconSet" priority="19">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5610,31 +6062,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53:I53">
-    <cfRule type="expression" dxfId="15" priority="17">
-      <formula>$G53=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="18">
-      <formula>$G53=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B53">
-    <cfRule type="expression" dxfId="13" priority="15">
-      <formula>$G53=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="16">
-      <formula>$G53=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
-    <cfRule type="expression" dxfId="11" priority="13">
-      <formula>$G54=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14">
-      <formula>$G54=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G54">
+  <conditionalFormatting sqref="C56:I56">
+    <cfRule type="expression" dxfId="31" priority="17">
+      <formula>$G56=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="18">
+      <formula>$G56=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B56">
+    <cfRule type="expression" dxfId="27" priority="15">
+      <formula>$G56=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="16">
+      <formula>$G56=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57">
+    <cfRule type="expression" dxfId="23" priority="13">
+      <formula>$G57=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="14">
+      <formula>$G57=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G57">
     <cfRule type="iconSet" priority="12">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5643,31 +6095,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54:I54">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>$G54=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="11">
-      <formula>$G54=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B54">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>$G54=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
-      <formula>$G54=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>$G55=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7">
-      <formula>$G55=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G55">
+  <conditionalFormatting sqref="C57:I57">
+    <cfRule type="expression" dxfId="19" priority="10">
+      <formula>$G57=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="11">
+      <formula>$G57=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57">
+    <cfRule type="expression" dxfId="15" priority="8">
+      <formula>$G57=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="9">
+      <formula>$G57=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="expression" dxfId="11" priority="6">
+      <formula>$G58=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="7">
+      <formula>$G58=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G58">
     <cfRule type="iconSet" priority="5">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5676,20 +6128,20 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C55:I55">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>$G55=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$G55=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B55">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$G55=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>$G55=2</formula>
+  <conditionalFormatting sqref="C58:I58">
+    <cfRule type="expression" dxfId="7" priority="3">
+      <formula>$G58=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="4">
+      <formula>$G58=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$G58=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$G58=2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Backup dos fontes 12/07/2013
</commit_message>
<xml_diff>
--- a/Acompanhamento de tarefas.xlsx
+++ b/Acompanhamento de tarefas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="180">
   <si>
     <t>Tarefas CCBA</t>
   </si>
@@ -556,6 +556,9 @@
   </si>
   <si>
     <t xml:space="preserve">CRIAR UM CONTROLE DE LOG PARA CADASTRO DE CLIENTES, DETALHANDO COM USUÁRIO QUE FEZ A ALTERAÇÃO, DATA E HORA, AÇÃO QUE FOI TOMADA </t>
+  </si>
+  <si>
+    <t>EM VALIDAÇÃO 05/07/2013</t>
   </si>
 </sst>
 </file>
@@ -3036,11 +3039,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan1"/>
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
+      <pane ySplit="5" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3057,7 +3060,7 @@
     <col min="11" max="16384" width="9.140625" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
       <c r="D1" s="57"/>
@@ -3067,7 +3070,7 @@
       <c r="H1" s="57"/>
       <c r="I1" s="57"/>
     </row>
-    <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="58"/>
       <c r="B2" s="81" t="s">
         <v>84</v>
@@ -3088,7 +3091,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="58"/>
       <c r="B3" s="58"/>
       <c r="C3" s="58"/>
@@ -3107,7 +3110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H4" s="59">
         <v>0</v>
       </c>
@@ -3119,7 +3122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="61" t="s">
         <v>5</v>
       </c>
@@ -3148,7 +3151,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="65">
         <v>1</v>
       </c>
@@ -3177,7 +3180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="65">
         <f t="shared" ref="A7:A12" si="0">A6+1</f>
         <v>2</v>
@@ -3207,7 +3210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A8" s="65">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3237,7 +3240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A9" s="65">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3267,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A10" s="65">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3297,7 +3300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A11" s="65">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3327,7 +3330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="65">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3357,7 +3360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A13" s="65">
         <f t="shared" ref="A13" si="1">A12+1</f>
         <v>8</v>
@@ -3387,7 +3390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A14" s="65">
         <f>A13+1</f>
         <v>9</v>
@@ -3414,8 +3417,11 @@
       <c r="I14" s="71">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="K14" s="80" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A15" s="65">
         <f>A14+1</f>
         <v>10</v>
@@ -3443,7 +3449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A16" s="65">
         <f>A15+1</f>
         <v>11</v>

</xml_diff>